<commit_message>
changed spreadsheet data to be more readable
</commit_message>
<xml_diff>
--- a/src/test/resources/asym-spreadsheet.xlsx
+++ b/src/test/resources/asym-spreadsheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -336,7 +336,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -373,300 +373,300 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>CONCATENATE("col", SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), " row", ROW())</f>
-        <v>colA row2</v>
+        <f>CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>A2</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:F2" si="1">CONCATENATE("col", SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), " row", ROW())</f>
-        <v>colB row2</v>
+        <f t="shared" ref="B2:F17" si="1">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>B2</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="1"/>
-        <v>colC row2</v>
+        <v>C2</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" si="1"/>
-        <v>colD row2</v>
+        <v>D2</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" si="1"/>
-        <v>colE row2</v>
+        <v>E2</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" si="1"/>
-        <v>colF row2</v>
+        <v>F2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:G19" si="2">CONCATENATE("col", SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), " row", ROW())</f>
-        <v>colA row3</v>
+        <f t="shared" ref="A3:G16" si="2">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>A3</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row3</v>
+        <f t="shared" si="1"/>
+        <v>B3</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row3</v>
+        <f t="shared" si="1"/>
+        <v>C3</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row3</v>
+        <f t="shared" si="1"/>
+        <v>D3</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row3</v>
+        <f t="shared" si="1"/>
+        <v>E3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="2"/>
-        <v>colA row4</v>
+        <v>A4</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row4</v>
+        <f t="shared" si="1"/>
+        <v>B4</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row4</v>
+        <f t="shared" si="1"/>
+        <v>D4</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row4</v>
+        <f t="shared" si="1"/>
+        <v>E4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="2"/>
-        <v>colA row5</v>
+        <v>A5</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row5</v>
+        <f t="shared" si="1"/>
+        <v>B5</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row5</v>
+        <f t="shared" si="1"/>
+        <v>C5</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row5</v>
+        <f t="shared" si="1"/>
+        <v>D5</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row5</v>
+        <f t="shared" si="1"/>
+        <v>E5</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="2"/>
-        <v>colF row5</v>
+        <f t="shared" si="1"/>
+        <v>F5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row6</v>
+        <f t="shared" si="1"/>
+        <v>B6</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row6</v>
+        <f t="shared" si="1"/>
+        <v>C6</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row6</v>
+        <f t="shared" si="1"/>
+        <v>D6</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row6</v>
+        <f t="shared" si="1"/>
+        <v>E6</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="2"/>
-        <v>colF row6</v>
+        <f t="shared" si="1"/>
+        <v>F6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f t="shared" si="2"/>
-        <v>colA row7</v>
+        <f>CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>A7</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row7</v>
+        <f t="shared" si="1"/>
+        <v>B7</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row7</v>
+        <f t="shared" si="1"/>
+        <v>C7</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row7</v>
+        <f>CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>D7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row8</v>
+        <f t="shared" si="1"/>
+        <v>B8</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row8</v>
+        <f t="shared" si="1"/>
+        <v>C8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f t="shared" si="2"/>
-        <v>colA row9</v>
+        <f t="shared" ref="A9:A12" si="3">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>A9</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row9</v>
+        <f t="shared" si="1"/>
+        <v>B9</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row9</v>
+        <f t="shared" si="1"/>
+        <v>C9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f t="shared" si="2"/>
-        <v>colA row10</v>
+        <f t="shared" si="3"/>
+        <v>A10</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row10</v>
+        <f t="shared" si="1"/>
+        <v>B10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f t="shared" si="2"/>
-        <v>colA row11</v>
+        <f t="shared" si="3"/>
+        <v>A11</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row11</v>
+        <f t="shared" si="1"/>
+        <v>B11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f t="shared" si="2"/>
-        <v>colA row12</v>
+        <f t="shared" si="3"/>
+        <v>A12</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row12</v>
+        <f t="shared" si="1"/>
+        <v>B12</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row12</v>
+        <f t="shared" ref="D12:G12" si="4">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>D12</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row12</v>
+        <f t="shared" si="4"/>
+        <v>E12</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
-        <v>colF row12</v>
+        <f t="shared" si="4"/>
+        <v>F12</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="2"/>
-        <v>colG row12</v>
+        <f t="shared" si="4"/>
+        <v>G12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row13</v>
+        <f t="shared" si="1"/>
+        <v>B13</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row13</v>
+        <f t="shared" si="1"/>
+        <v>C13</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row13</v>
+        <f t="shared" si="1"/>
+        <v>D13</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row13</v>
+        <f t="shared" si="1"/>
+        <v>E13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row14</v>
+        <f t="shared" si="1"/>
+        <v>B14</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row14</v>
+        <f t="shared" si="1"/>
+        <v>C14</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row14</v>
+        <f t="shared" si="1"/>
+        <v>D14</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row14</v>
+        <f t="shared" si="1"/>
+        <v>E14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row15</v>
+        <f t="shared" si="1"/>
+        <v>B15</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row15</v>
+        <f t="shared" si="1"/>
+        <v>C15</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row15</v>
+        <f t="shared" si="1"/>
+        <v>D15</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row15</v>
+        <f t="shared" si="1"/>
+        <v>E15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="str">
-        <f t="shared" si="2"/>
-        <v>colB row16</v>
+        <f t="shared" si="1"/>
+        <v>B16</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="2"/>
-        <v>colC row16</v>
+        <f t="shared" si="1"/>
+        <v>C16</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row16</v>
+        <f t="shared" si="1"/>
+        <v>D16</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="2"/>
-        <v>colE row16</v>
+        <f t="shared" si="1"/>
+        <v>E16</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row17</v>
+        <f t="shared" si="1"/>
+        <v>D17</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row18</v>
+        <f t="shared" ref="D18:D20" si="5">CONCATENATE(SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), ROW())</f>
+        <v>D18</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
-        <v>colD row19</v>
+        <f t="shared" si="5"/>
+        <v>D19</v>
       </c>
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" t="str">
-        <f t="shared" ref="D20" si="3">CONCATENATE("col", SUBSTITUTE(ADDRESS(1,COLUMN(),4),"1",""), " row", ROW())</f>
-        <v>colD row20</v>
+        <f t="shared" si="5"/>
+        <v>D20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>